<commit_message>
recommendation system is updated
</commit_message>
<xml_diff>
--- a/data/cleaned_data.xlsx
+++ b/data/cleaned_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Drive\CMIS 4†26 - Project\Data Set\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Drive\CMIS 4†26 - Project\Data Set\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC2BFC6-17BA-4437-8E39-69999B0F99E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B355EAF-FB5A-4225-B026-44FFD18A1FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -807,11 +807,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1116,17 +1117,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="BB1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BC1" sqref="BC1:BC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="13.44140625" customWidth="1"/>
     <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="27.77734375" customWidth="1"/>
+    <col min="9" max="9" width="23.77734375" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" customWidth="1"/>
+    <col min="11" max="11" width="28.77734375" customWidth="1"/>
+    <col min="12" max="12" width="29.6640625" customWidth="1"/>
+    <col min="13" max="13" width="34.6640625" customWidth="1"/>
+    <col min="14" max="14" width="39.109375" customWidth="1"/>
+    <col min="15" max="15" width="30.44140625" customWidth="1"/>
+    <col min="16" max="16" width="34.88671875" customWidth="1"/>
+    <col min="17" max="17" width="76.5546875" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" customWidth="1"/>
+    <col min="19" max="19" width="17.109375" customWidth="1"/>
+    <col min="20" max="20" width="20.77734375" customWidth="1"/>
+    <col min="21" max="21" width="28.33203125" customWidth="1"/>
+    <col min="22" max="22" width="32.33203125" customWidth="1"/>
+    <col min="23" max="23" width="21" customWidth="1"/>
+    <col min="24" max="24" width="26.33203125" customWidth="1"/>
+    <col min="25" max="25" width="29.33203125" customWidth="1"/>
+    <col min="26" max="26" width="36.6640625" customWidth="1"/>
+    <col min="27" max="27" width="28.5546875" customWidth="1"/>
+    <col min="28" max="28" width="43.44140625" customWidth="1"/>
+    <col min="29" max="29" width="28.6640625" customWidth="1"/>
+    <col min="30" max="30" width="26.109375" customWidth="1"/>
+    <col min="31" max="31" width="22.109375" customWidth="1"/>
+    <col min="32" max="32" width="22.77734375" customWidth="1"/>
+    <col min="33" max="33" width="21.44140625" customWidth="1"/>
+    <col min="34" max="34" width="22.44140625" customWidth="1"/>
+    <col min="35" max="35" width="20.44140625" customWidth="1"/>
+    <col min="36" max="36" width="21" customWidth="1"/>
+    <col min="37" max="37" width="20.77734375" customWidth="1"/>
+    <col min="38" max="38" width="18.77734375" customWidth="1"/>
+    <col min="39" max="39" width="19.33203125" customWidth="1"/>
+    <col min="40" max="40" width="32.5546875" customWidth="1"/>
+    <col min="41" max="41" width="27.33203125" customWidth="1"/>
+    <col min="42" max="42" width="26.109375" customWidth="1"/>
+    <col min="43" max="43" width="22.109375" customWidth="1"/>
+    <col min="44" max="44" width="19" customWidth="1"/>
+    <col min="45" max="45" width="24.44140625" customWidth="1"/>
+    <col min="46" max="46" width="23.33203125" customWidth="1"/>
+    <col min="47" max="47" width="23.21875" customWidth="1"/>
+    <col min="48" max="48" width="20.5546875" customWidth="1"/>
+    <col min="49" max="49" width="25.33203125" customWidth="1"/>
+    <col min="50" max="50" width="31.109375" customWidth="1"/>
+    <col min="51" max="51" width="30.21875" customWidth="1"/>
+    <col min="52" max="52" width="24.21875" customWidth="1"/>
+    <col min="53" max="53" width="24.33203125" customWidth="1"/>
+    <col min="54" max="54" width="17.88671875" customWidth="1"/>
+    <col min="55" max="55" width="20.44140625" customWidth="1"/>
+    <col min="56" max="56" width="40" customWidth="1"/>
+    <col min="57" max="57" width="23.6640625" customWidth="1"/>
+    <col min="58" max="58" width="12.88671875" customWidth="1"/>
+    <col min="59" max="59" width="21.21875" customWidth="1"/>
+    <col min="60" max="60" width="16.44140625" customWidth="1"/>
+    <col min="61" max="61" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:61" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -67185,5 +67240,6 @@
   </sheetData>
   <autoFilter ref="G1:G364" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>